<commit_message>
correction - Mathis fait
</commit_message>
<xml_diff>
--- a/LabsGrilleDeCorrection.xlsx
+++ b/LabsGrilleDeCorrection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab4 - Vanderlay Industries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab4 - Vanderlay Industries/Groupe4/Lab4-VanderlayIndustries-G4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ABA8C1F-5A35-4B06-9FA2-560DF65F3C33}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE244E4-BD58-4F88-83F3-0C78102552FF}"/>
   <bookViews>
-    <workbookView xWindow="4212" yWindow="3060" windowWidth="17280" windowHeight="8880" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
+    <workbookView xWindow="-56535" yWindow="3225" windowWidth="19215" windowHeight="19650" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Exigences</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>La grille de planification est remplise et décrit bien les nécessitées de l'entreprise</t>
+  </si>
+  <si>
+    <t>Attention: logo de page de produit est déformé</t>
+  </si>
+  <si>
+    <t>préférable de centrer les produits, au lieu de laisser 3/4 de la page vide</t>
+  </si>
+  <si>
+    <t>manque une section de jobs pour George</t>
+  </si>
+  <si>
+    <t>bon commentaires bien utile en html, mais manque de commentaires en css</t>
   </si>
 </sst>
 </file>
@@ -452,17 +464,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13015D56-4554-4253-AD0C-2910E2AEE6AE}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,119 +488,183 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -598,67 +674,67 @@
       </c>
       <c r="C16">
         <f>SUM(C2:C15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17">
         <f>C16/B16*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102.8301886792453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
   </sheetData>

</xml_diff>